<commit_message>
Added notes on next analyses
</commit_message>
<xml_diff>
--- a/tables/bael_analysis_tables_151028.xlsx
+++ b/tables/bael_analysis_tables_151028.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13940" yWindow="1820" windowWidth="21620" windowHeight="16120" tabRatio="500"/>
+    <workbookView xWindow="14620" yWindow="4360" windowWidth="15360" windowHeight="15760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AIC" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
   <si>
     <t>Modnames</t>
   </si>
@@ -199,6 +199,522 @@
   </si>
   <si>
     <r>
+      <t>Growth (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>g</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">', </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>' = 0.21 + 0.78</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>; σ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> = 0.11</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Recruit size (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>recruit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>recruit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> = 0.14; σ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">  = 0.07</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>recruit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> = 0.16; σ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">  = 0.09</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Size at maturity (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>mat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>mat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> = 0.39</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Embryo number (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> = -16.29 + 41.61</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">z; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>σ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> = 0.3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Recruitment probability (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>recruit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>recruit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> = 0.074; σ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">  = 0.076</t>
+    </r>
+  </si>
+  <si>
+    <t>Size (full dataset)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>' = 0.20 + 0.87</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>; σ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> = 0.10</t>
+    </r>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <r>
       <t>logit(</t>
     </r>
     <r>
@@ -216,7 +732,7 @@
         <color theme="1"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t>) = 1.71 + 0.78</t>
+      <t>) = 1.71 + 0.45</t>
     </r>
     <r>
       <rPr>
@@ -229,520 +745,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Growth (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>g</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>z</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">', </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>z</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>))</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>z</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>' = 0.21 + 0.78</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>z</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>; σ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> = 0.11</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Recruit size (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>z</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>recruit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>z</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>recruit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> = 0.14; σ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">  = 0.07</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>z</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>recruit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> = 0.16; σ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">  = 0.09</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Size at maturity (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>z</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>mat</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>z</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>mat</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> = 0.39</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Embryo number (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>z</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>))</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> = -16.29 + 41.61</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">z; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>σ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> = 0.3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Recruitment probability (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>p</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>recruit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>p</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>recruit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> = 0.074; σ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">  = 0.076</t>
-    </r>
-  </si>
-  <si>
-    <t>Size (full dataset)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>z</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>' = 0.20 + 0.87</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>z</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>; σ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> = 0.10</t>
-    </r>
-  </si>
-  <si>
-    <t>Density</t>
+    <t>updated: 3 Dec 2015</t>
   </si>
 </sst>
 </file>
@@ -1418,8 +1421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11:R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1656,7 +1659,7 @@
       <c r="H6"/>
       <c r="I6"/>
       <c r="K6" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
@@ -2637,7 +2640,7 @@
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L31" s="8"/>
       <c r="M31" s="8"/>
@@ -2801,10 +2804,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2841,12 +2844,12 @@
         <v>27</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="16"/>
     </row>
@@ -2855,7 +2858,7 @@
         <v>26</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2863,12 +2866,12 @@
         <v>27</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17">
       <c r="A8" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="16"/>
     </row>
@@ -2877,7 +2880,7 @@
         <v>26</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17">
@@ -2885,31 +2888,36 @@
         <v>27</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="17">
       <c r="A11" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>37</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="16" t="s">
         <v>39</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="17">
       <c r="A13" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>42</v>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="15" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>